<commit_message>
New Link image Logo Banks
</commit_message>
<xml_diff>
--- a/AuxTable_Ticker_Logo.xlsx
+++ b/AuxTable_Ticker_Logo.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\yFinance_BI_2.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\__GitHub\yFinance_BI_2.0_TEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BE178F-FF4F-431D-A327-2A4D8A6CC080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18255C5D-7A63-4B86-A8C3-C4FAB532135D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{24FF7FC9-2181-4C35-B5DC-4E251A4B7CC5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabela Auxiliar" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,9 +42,6 @@
     <t>link_logo</t>
   </si>
   <si>
-    <t>yFinance_BI_2.0_TEST/Assets/Banco Itaú/ITUB4_Logo.svg at master · Mateus-Fleck/yFinance_BI_2.0_TEST (github.com)</t>
-  </si>
-  <si>
     <t>ITUB4</t>
   </si>
   <si>
@@ -57,15 +54,6 @@
     <t>CXSE3</t>
   </si>
   <si>
-    <t>yFinance_BI_2.0_TEST/Assets/Banco do Brasil/BBAS3_Logo.svg at master · Mateus-Fleck/yFinance_BI_2.0_TEST (github.com)</t>
-  </si>
-  <si>
-    <t>yFinance_BI_2.0_TEST/Assets/Brasil Bolsa Balcão/B3SA3_logo.svg at master · Mateus-Fleck/yFinance_BI_2.0_TEST (github.com)</t>
-  </si>
-  <si>
-    <t>yFinance_BI_2.0_TEST/Assets/CaixaEconomica/CXSE3_Logo.svg at master · Mateus-Fleck/yFinance_BI_2.0_TEST (github.com)</t>
-  </si>
-  <si>
     <t>nome</t>
   </si>
   <si>
@@ -79,6 +67,18 @@
   </si>
   <si>
     <t>Caixa Econômica Federal</t>
+  </si>
+  <si>
+    <t>https://github.com/Mateus-Fleck/yFinance_BI_2.0_TEST/blob/main/Assets/Banco%20do%20Brasil/BBAS3_Logo.png</t>
+  </si>
+  <si>
+    <t>https://github.com/Mateus-Fleck/yFinance_BI_2.0_TEST/blob/main/Assets/Banco%20Ita%C3%BA/ITUB4_Logo.png</t>
+  </si>
+  <si>
+    <t>https://github.com/Mateus-Fleck/yFinance_BI_2.0_TEST/blob/main/Assets/Brasil%20Bolsa%20Balc%C3%A3o/B3SA3_Logo.png</t>
+  </si>
+  <si>
+    <t>https://github.com/Mateus-Fleck/yFinance_BI_2.0_TEST/blob/main/Assets/CaixaEconomica/CXSE3_Logo.png</t>
   </si>
 </sst>
 </file>
@@ -150,7 +150,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -161,6 +161,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -548,7 +549,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -564,7 +565,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -572,61 +573,65 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>2</v>
+        <v>9</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>9</v>
-      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C7" s="5"/>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C20" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" display="https://github.com/Mateus-Fleck/yFinance_BI_2.0_TEST/blob/master/Assets/Banco Ita%C3%BA/ITUB4_Logo.svg" xr:uid="{85020393-9912-4DC0-8B49-E6FE04973B1F}"/>
-    <hyperlink ref="C3" r:id="rId2" display="https://github.com/Mateus-Fleck/yFinance_BI_2.0_TEST/blob/master/Assets/Banco do Brasil/BBAS3_Logo.svg" xr:uid="{BA1C841C-D063-4691-A4A4-70DE82A04D86}"/>
-    <hyperlink ref="C2" r:id="rId3" display="https://github.com/Mateus-Fleck/yFinance_BI_2.0_TEST/blob/master/Assets/Brasil Bolsa Balc%C3%A3o/B3SA3_logo.svg" xr:uid="{4BDE98D8-A4F3-4F43-ACEB-F4FA86200E37}"/>
-    <hyperlink ref="C5" r:id="rId4" display="https://github.com/Mateus-Fleck/yFinance_BI_2.0_TEST/blob/master/Assets/CaixaEconomica/CXSE3_Logo.svg" xr:uid="{83B7150D-F688-4ED4-AC59-6A938AE58EBA}"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{BA1C841C-D063-4691-A4A4-70DE82A04D86}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{4BDE98D8-A4F3-4F43-ACEB-F4FA86200E37}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{83B7150D-F688-4ED4-AC59-6A938AE58EBA}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{2592C901-4F88-4992-958C-435EE053B9AE}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualizacao do Projeto,Update Layout
</commit_message>
<xml_diff>
--- a/AuxTable_Ticker_Logo.xlsx
+++ b/AuxTable_Ticker_Logo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\__GitHub\yFinance_BI_2.0_TEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18255C5D-7A63-4B86-A8C3-C4FAB532135D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489F41E4-17FF-4BFF-9DF9-5FD53E31D90C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{24FF7FC9-2181-4C35-B5DC-4E251A4B7CC5}"/>
   </bookViews>
@@ -34,13 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>ticker</t>
-  </si>
-  <si>
-    <t>link_logo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>ITUB4</t>
   </si>
@@ -54,9 +48,6 @@
     <t>CXSE3</t>
   </si>
   <si>
-    <t>nome</t>
-  </si>
-  <si>
     <t>Banco do Brasil</t>
   </si>
   <si>
@@ -69,16 +60,40 @@
     <t>Caixa Econômica Federal</t>
   </si>
   <si>
+    <t>https://drive.google.com/file/d/1uSfi9gF1oyq2Lj1pdqqgOJsMGbhvpTYE/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1tgS1_skpbQs4ThAT-mgCcoodwGHBBBJI/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/13wZrLar4IFXM2M36TpnYxPisyyhxYUhV/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1KuxPtlEWHyFxcgSoEWEmCvFuViFGO34X/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>https://github.com/Mateus-Fleck/yFinance_BI_2.0_TEST/blob/main/Assets/Banco%20Ita%C3%BA/ITUB4_Logo.png</t>
+  </si>
+  <si>
     <t>https://github.com/Mateus-Fleck/yFinance_BI_2.0_TEST/blob/main/Assets/Banco%20do%20Brasil/BBAS3_Logo.png</t>
   </si>
   <si>
-    <t>https://github.com/Mateus-Fleck/yFinance_BI_2.0_TEST/blob/main/Assets/Banco%20Ita%C3%BA/ITUB4_Logo.png</t>
-  </si>
-  <si>
     <t>https://github.com/Mateus-Fleck/yFinance_BI_2.0_TEST/blob/main/Assets/Brasil%20Bolsa%20Balc%C3%A3o/B3SA3_Logo.png</t>
   </si>
   <si>
     <t>https://github.com/Mateus-Fleck/yFinance_BI_2.0_TEST/blob/main/Assets/CaixaEconomica/CXSE3_Logo.png</t>
+  </si>
+  <si>
+    <t>Link_Logo_GitHub</t>
+  </si>
+  <si>
+    <t>Link_Logo_Google_Drive2</t>
+  </si>
+  <si>
+    <t>Ticker</t>
+  </si>
+  <si>
+    <t>Nome_Acao</t>
   </si>
 </sst>
 </file>
@@ -150,7 +165,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -162,6 +177,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -238,12 +255,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{12D60882-A40E-42C8-A21B-B2C68E62F366}" name="Tabela1" displayName="Tabela1" ref="A1:C5" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
-  <autoFilter ref="A1:C5" xr:uid="{12D60882-A40E-42C8-A21B-B2C68E62F366}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{24E937F5-AA76-44E5-A81F-C797A3EB2942}" name="ticker" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{0D998ECA-C8B1-4827-A5DA-8A7B3EA460A4}" name="nome"/>
-    <tableColumn id="2" xr3:uid="{FB45F293-2B5E-4541-B41E-F487493923A1}" name="link_logo" dataDxfId="0" dataCellStyle="Hiperlink"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{12D60882-A40E-42C8-A21B-B2C68E62F366}" name="Tabela1" displayName="Tabela1" ref="A1:D5" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="A1:D5" xr:uid="{12D60882-A40E-42C8-A21B-B2C68E62F366}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{24E937F5-AA76-44E5-A81F-C797A3EB2942}" name="Ticker" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{0D998ECA-C8B1-4827-A5DA-8A7B3EA460A4}" name="Nome_Acao"/>
+    <tableColumn id="4" xr3:uid="{84844451-83F0-4C7B-A12B-203EEA756E46}" name="Link_Logo_GitHub"/>
+    <tableColumn id="2" xr3:uid="{FB45F293-2B5E-4541-B41E-F487493923A1}" name="Link_Logo_Google_Drive2" dataDxfId="0" dataCellStyle="Hiperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -546,87 +564,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{420E87B5-D8C4-4448-AC9C-FCD0C559585B}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="107.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="107.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="107.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B4" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C7" s="5"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C20" s="5"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D7" s="5"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D11" s="5"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C16" s="5"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D21" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{BA1C841C-D063-4691-A4A4-70DE82A04D86}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{4BDE98D8-A4F3-4F43-ACEB-F4FA86200E37}"/>
-    <hyperlink ref="C5" r:id="rId3" xr:uid="{83B7150D-F688-4ED4-AC59-6A938AE58EBA}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{2592C901-4F88-4992-958C-435EE053B9AE}"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{9F4E9E8C-2644-477A-826F-444C3FF9E5E0}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{E0E98C1D-EB00-43C2-BDFD-0928924AC251}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{B5F9969B-D070-47E3-9FBF-813BFF907004}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{BD3E90F3-09A9-473F-B570-43D321976DA1}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>

</xml_diff>